<commit_message>
Main loop reads RTC clock and prints out to serial
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834869BF-1902-47D2-B7EA-1ACA8AA9EB6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E724DD8-2CAD-41BB-9543-4A7E5295AEC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>Frame</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Required </t>
   </si>
   <si>
     <t>Development Phase</t>
@@ -435,6 +432,12 @@
   </si>
   <si>
     <t>SPI</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Required (days) </t>
   </si>
 </sst>
 </file>
@@ -911,7 +914,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1115,19 +1118,20 @@
     <xf numFmtId="166" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="7" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="20" xfId="8" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="21" xfId="8" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="7" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Date" xfId="4" xr:uid="{BF5E08F0-45D4-4B89-9CAF-52F8DB1B8960}"/>
@@ -1517,13 +1521,13 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="42.44140625" customWidth="1"/>
@@ -1532,10 +1536,10 @@
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
@@ -1551,7 +1555,10 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="80">
+        <f>ProjectSchedule!F11-ProjectSchedule!E9</f>
+        <v>36</v>
+      </c>
       <c r="C3" s="3">
         <v>43956</v>
       </c>
@@ -1562,14 +1569,17 @@
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f>ProjectSchedule!F16-ProjectSchedule!E13</f>
+        <v>31</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>1</v>
@@ -1577,42 +1587,42 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1628,9 +1638,9 @@
   </sheetPr>
   <dimension ref="A1:CH21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1654,10 +1664,10 @@
   <sheetData>
     <row r="1" spans="1:86" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="63" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" s="63" t="s">
-        <v>44</v>
       </c>
       <c r="C1" s="62"/>
       <c r="D1" s="59"/>
@@ -1665,44 +1675,44 @@
       <c r="F1" s="60"/>
       <c r="H1" s="59"/>
       <c r="I1" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:86" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:86" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="75">
+        <v>45</v>
+      </c>
+      <c r="C3" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="76"/>
+      <c r="E3" s="78">
         <v>43956</v>
       </c>
-      <c r="F3" s="76"/>
+      <c r="F3" s="79"/>
     </row>
     <row r="4" spans="1:86" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="C4" s="75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="76"/>
       <c r="E4" s="55">
         <v>1</v>
       </c>
@@ -1819,14 +1829,14 @@
     </row>
     <row r="5" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
+        <v>34</v>
+      </c>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
       <c r="I5" s="54">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43955</v>
@@ -2140,28 +2150,28 @@
         <v>44032</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:86" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="50"/>
       <c r="H6" s="50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="49" t="str">
         <f t="shared" ref="I6:AN6" si="11">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2476,9 +2486,9 @@
         <v>M</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:86" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8"/>
       <c r="E7"/>
@@ -2567,10 +2577,10 @@
     </row>
     <row r="8" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="47"/>
       <c r="D8" s="46"/>
@@ -2662,16 +2672,16 @@
     </row>
     <row r="9" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="41">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="E9" s="40">
         <f>Project_Start</f>
@@ -2767,13 +2777,13 @@
     </row>
     <row r="10" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>75</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>76</v>
       </c>
       <c r="D10" s="41">
         <v>0</v>
@@ -2873,10 +2883,10 @@
     <row r="11" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14"/>
       <c r="B11" s="43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="41">
         <v>0</v>
@@ -2975,7 +2985,7 @@
     </row>
     <row r="12" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="39" t="s">
         <v>1</v>
@@ -3071,10 +3081,10 @@
     <row r="13" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="31">
         <v>0</v>
@@ -3174,10 +3184,10 @@
     <row r="14" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="31">
         <v>0</v>
@@ -3277,10 +3287,10 @@
     <row r="15" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="31">
         <v>0</v>
@@ -3380,10 +3390,10 @@
     <row r="16" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="31">
         <v>0</v>
@@ -3482,10 +3492,10 @@
     </row>
     <row r="17" spans="1:86" s="19" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="24"/>
@@ -3772,10 +3782,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47672CA-176D-4AFA-9F31-8EFAC836D0A5}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3786,144 +3796,159 @@
     <col min="5" max="5" width="51.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A9" si="0">ROW()-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <f>SUM(D2:D9)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
@@ -3949,13 +3974,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3963,7 +3988,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3974,7 +3999,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -3985,7 +4010,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -3996,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -4007,7 +4032,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4018,7 +4043,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4029,7 +4054,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4040,7 +4065,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -4051,7 +4076,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -4062,7 +4087,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -4073,7 +4098,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -4081,7 +4106,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13">
         <f>SUM(D2:D12)</f>
@@ -4110,21 +4135,21 @@
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -4132,10 +4157,10 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -4143,10 +4168,10 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -4154,10 +4179,10 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -4165,10 +4190,10 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4176,10 +4201,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4187,10 +4212,10 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -4198,7 +4223,7 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9">
         <f>SUM(D2:D8)</f>
@@ -4243,42 +4268,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
       <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="H1" t="s">
-        <v>107</v>
-      </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
         <v>95</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>96</v>
       </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2">
         <v>115200</v>
@@ -4286,19 +4311,19 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
         <v>98</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>99</v>
       </c>
-      <c r="C3" t="s">
-        <v>100</v>
-      </c>
       <c r="G3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I3">
         <v>19200</v>
@@ -4306,19 +4331,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" t="s">
-        <v>102</v>
-      </c>
       <c r="G4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I4">
         <v>400000</v>
@@ -4326,19 +4351,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="B5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C5" t="s">
-        <v>104</v>
-      </c>
       <c r="G5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I5">
         <v>3250000</v>
@@ -4346,10 +4371,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I6">
         <v>3250000</v>
@@ -4357,10 +4382,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I7">
         <v>400000</v>

</xml_diff>

<commit_message>
Added Periodic Wake Up
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E724DD8-2CAD-41BB-9543-4A7E5295AEC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D959CF1-633C-4406-8F32-DE44D2842039}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
   <si>
     <t>Frame</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t xml:space="preserve">Time Required (days) </t>
+  </si>
+  <si>
+    <t>Configure Pins for PWR shutdown/stop mode</t>
   </si>
 </sst>
 </file>
@@ -1109,6 +1112,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1131,7 +1135,6 @@
     <xf numFmtId="167" fontId="1" fillId="0" borderId="21" xfId="8" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Date" xfId="4" xr:uid="{BF5E08F0-45D4-4B89-9CAF-52F8DB1B8960}"/>
@@ -1555,9 +1558,9 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="80">
+      <c r="B3" s="72">
         <f>ProjectSchedule!F11-ProjectSchedule!E9</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="3">
         <v>43956</v>
@@ -1640,7 +1643,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1696,147 +1699,147 @@
       <c r="B3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="78">
+      <c r="D3" s="77"/>
+      <c r="E3" s="79">
         <v>43956</v>
       </c>
-      <c r="F3" s="79"/>
+      <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:86" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="76"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="55">
         <v>1</v>
       </c>
-      <c r="I4" s="72">
+      <c r="I4" s="73">
         <f>I5</f>
         <v>43955</v>
       </c>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="72">
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="73">
         <f>P5</f>
         <v>43962</v>
       </c>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="74"/>
-      <c r="W4" s="72">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="73">
         <f>W5</f>
         <v>43969</v>
       </c>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
-      <c r="Z4" s="73"/>
-      <c r="AA4" s="73"/>
-      <c r="AB4" s="73"/>
-      <c r="AC4" s="74"/>
-      <c r="AD4" s="72">
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="73">
         <f>AD5</f>
         <v>43976</v>
       </c>
-      <c r="AE4" s="73"/>
-      <c r="AF4" s="73"/>
-      <c r="AG4" s="73"/>
-      <c r="AH4" s="73"/>
-      <c r="AI4" s="73"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="72">
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="73">
         <f>AK5</f>
         <v>43983</v>
       </c>
-      <c r="AL4" s="73"/>
-      <c r="AM4" s="73"/>
-      <c r="AN4" s="73"/>
-      <c r="AO4" s="73"/>
-      <c r="AP4" s="73"/>
-      <c r="AQ4" s="74"/>
-      <c r="AR4" s="72">
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="74"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="73">
         <f>AR5</f>
         <v>43990</v>
       </c>
-      <c r="AS4" s="73"/>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="74"/>
-      <c r="AY4" s="72">
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="74"/>
+      <c r="AU4" s="74"/>
+      <c r="AV4" s="74"/>
+      <c r="AW4" s="74"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="73">
         <f>AY5</f>
         <v>43997</v>
       </c>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="74"/>
-      <c r="BF4" s="72">
+      <c r="AZ4" s="74"/>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="74"/>
+      <c r="BC4" s="74"/>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="73">
         <f>BF5</f>
         <v>44004</v>
       </c>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="73"/>
-      <c r="BL4" s="74"/>
-      <c r="BM4" s="72">
+      <c r="BG4" s="74"/>
+      <c r="BH4" s="74"/>
+      <c r="BI4" s="74"/>
+      <c r="BJ4" s="74"/>
+      <c r="BK4" s="74"/>
+      <c r="BL4" s="75"/>
+      <c r="BM4" s="73">
         <f>BM5</f>
         <v>44011</v>
       </c>
-      <c r="BN4" s="73"/>
-      <c r="BO4" s="73"/>
-      <c r="BP4" s="73"/>
-      <c r="BQ4" s="73"/>
-      <c r="BR4" s="73"/>
-      <c r="BS4" s="74"/>
-      <c r="BT4" s="72">
+      <c r="BN4" s="74"/>
+      <c r="BO4" s="74"/>
+      <c r="BP4" s="74"/>
+      <c r="BQ4" s="74"/>
+      <c r="BR4" s="74"/>
+      <c r="BS4" s="75"/>
+      <c r="BT4" s="73">
         <f>BT5</f>
         <v>44018</v>
       </c>
-      <c r="BU4" s="73"/>
-      <c r="BV4" s="73"/>
-      <c r="BW4" s="73"/>
-      <c r="BX4" s="73"/>
-      <c r="BY4" s="73"/>
-      <c r="BZ4" s="74"/>
-      <c r="CB4" s="72">
+      <c r="BU4" s="74"/>
+      <c r="BV4" s="74"/>
+      <c r="BW4" s="74"/>
+      <c r="BX4" s="74"/>
+      <c r="BY4" s="74"/>
+      <c r="BZ4" s="75"/>
+      <c r="CB4" s="73">
         <f>CB5</f>
         <v>44026</v>
       </c>
-      <c r="CC4" s="73"/>
-      <c r="CD4" s="73"/>
-      <c r="CE4" s="73"/>
-      <c r="CF4" s="73"/>
-      <c r="CG4" s="73"/>
-      <c r="CH4" s="74"/>
+      <c r="CC4" s="74"/>
+      <c r="CD4" s="74"/>
+      <c r="CE4" s="74"/>
+      <c r="CF4" s="74"/>
+      <c r="CG4" s="74"/>
+      <c r="CH4" s="75"/>
     </row>
     <row r="5" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
       <c r="I5" s="54">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43955</v>
@@ -2786,20 +2789,20 @@
         <v>75</v>
       </c>
       <c r="D10" s="41">
-        <v>0</v>
+        <v>0.2727</v>
       </c>
       <c r="E10" s="40">
         <f>F9+1</f>
         <v>43965</v>
       </c>
       <c r="F10" s="40">
-        <f>E10+'Power Mode Config'!D13</f>
-        <v>43976</v>
+        <f>E10+'Power Mode Config'!D14</f>
+        <v>43977</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="29">
         <f t="shared" si="28"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
@@ -2893,11 +2896,11 @@
       </c>
       <c r="E11" s="40">
         <f>F10+1</f>
-        <v>43977</v>
+        <v>43978</v>
       </c>
       <c r="F11" s="40">
         <f>E11+'State Machine'!D9</f>
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="29">
@@ -3091,11 +3094,11 @@
       </c>
       <c r="E13" s="30">
         <f>F11+1</f>
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="F13" s="30">
         <f>E13+7</f>
-        <v>44000</v>
+        <v>44001</v>
       </c>
       <c r="G13" s="29"/>
       <c r="H13" s="29">
@@ -3194,11 +3197,11 @@
       </c>
       <c r="E14" s="30">
         <f>F13+1</f>
-        <v>44001</v>
+        <v>44002</v>
       </c>
       <c r="F14" s="30">
         <f>E14+7</f>
-        <v>44008</v>
+        <v>44009</v>
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="29">
@@ -3297,11 +3300,11 @@
       </c>
       <c r="E15" s="30">
         <f>F14+1</f>
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="F15" s="30">
         <f>E15+7</f>
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="G15" s="29"/>
       <c r="H15" s="29">
@@ -3400,11 +3403,11 @@
       </c>
       <c r="E16" s="30">
         <f>F15+1</f>
-        <v>44017</v>
+        <v>44018</v>
       </c>
       <c r="F16" s="30">
         <f>E16+7</f>
-        <v>44024</v>
+        <v>44025</v>
       </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29">
@@ -3752,7 +3755,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="91" fitToWidth="2" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="86" fitToWidth="2" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -3960,10 +3963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F1D85-7517-4754-91FA-550EA766F607}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3972,7 +3975,7 @@
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>17</v>
       </c>
@@ -3983,7 +3986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3994,7 +3997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4005,7 +4008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4016,7 +4019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4027,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4037,8 +4040,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4048,8 +4054,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4059,58 +4068,69 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
+      <c r="E8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
         <v>76</v>
       </c>
-      <c r="D13">
-        <f>SUM(D2:D12)</f>
-        <v>11</v>
+      <c r="D14">
+        <f>SUM(D2:D13)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Software Reset Handler
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D959CF1-633C-4406-8F32-DE44D2842039}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D3953C-094C-402A-A758-B9707C2B5170}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
   <si>
     <t>Frame</t>
   </si>
@@ -1643,7 +1643,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2684,7 +2684,7 @@
         <v>75</v>
       </c>
       <c r="D9" s="41">
-        <v>0.63</v>
+        <v>0.88</v>
       </c>
       <c r="E9" s="40">
         <f>Project_Start</f>
@@ -2789,7 +2789,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="41">
-        <v>0.2727</v>
+        <v>0.5</v>
       </c>
       <c r="E10" s="40">
         <f>F9+1</f>
@@ -3963,178 +3963,186 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F1D85-7517-4754-91FA-550EA766F607}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D2">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D3">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D4">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D5">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D6">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D8">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D9">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D13">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <f>SUM(D2:D13)</f>
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Transitions to Transmit State
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D3953C-094C-402A-A758-B9707C2B5170}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B530B3-123F-4F9E-8E82-E0FF9BAB0033}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
@@ -1641,9 +1641,9 @@
   </sheetPr>
   <dimension ref="A1:CH21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2789,7 +2789,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="41">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="40">
         <f>F9+1</f>
@@ -2892,7 +2892,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="41">
-        <v>0</v>
+        <v>0.33329999999999999</v>
       </c>
       <c r="E11" s="40">
         <f>F10+1</f>
@@ -3744,7 +3744,7 @@
       <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -4151,54 +4151,55 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>86</v>
       </c>
       <c r="D4">
@@ -4206,10 +4207,10 @@
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D5">
@@ -4217,10 +4218,10 @@
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D6">
@@ -4228,21 +4229,21 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="8" t="s">
         <v>89</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="8" t="s">
         <v>90</v>
       </c>
       <c r="D8">
@@ -4250,7 +4251,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+      <c r="C9" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D9">
@@ -4260,6 +4261,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Buoy Framework Development Plan.xlsx
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B530B3-123F-4F9E-8E82-E0FF9BAB0033}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A90EDF3-7D8F-4C2E-918C-552620761BBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
@@ -1641,9 +1641,9 @@
   </sheetPr>
   <dimension ref="A1:CH21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2892,7 +2892,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="41">
-        <v>0.33329999999999999</v>
+        <v>0.66669999999999996</v>
       </c>
       <c r="E11" s="40">
         <f>F10+1</f>

</xml_diff>

<commit_message>
made library more portable
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB6DCB-D34D-4DC1-8F5C-58AFDC93000F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD89A0-FE2A-4203-BF1C-FF9F6132A101}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="137">
   <si>
     <t>Frame</t>
   </si>
@@ -474,6 +474,24 @@
   </si>
   <si>
     <t>Pin Map</t>
+  </si>
+  <si>
+    <t>Data Flash</t>
+  </si>
+  <si>
+    <t>Create Init Function</t>
+  </si>
+  <si>
+    <t>Create flow chart for routine</t>
+  </si>
+  <si>
+    <t>Save Data</t>
+  </si>
+  <si>
+    <t>Load Data</t>
+  </si>
+  <si>
+    <t>Create memory map</t>
   </si>
 </sst>
 </file>
@@ -1676,9 +1694,9 @@
   </sheetPr>
   <dimension ref="A1:CH21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2927,7 +2945,7 @@
         <v>75</v>
       </c>
       <c r="D11" s="41">
-        <v>0.66669999999999996</v>
+        <v>1</v>
       </c>
       <c r="E11" s="40">
         <f>F10+1</f>
@@ -3125,7 +3143,7 @@
         <v>75</v>
       </c>
       <c r="D13" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="30">
         <f>F11+1</f>
@@ -4302,15 +4320,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C443201F-21B9-4781-9C9F-956B668549C5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4374,6 +4392,36 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Synthesis of GPS and MEM
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD89A0-FE2A-4203-BF1C-FF9F6132A101}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB84021-22F5-4DCE-A211-D0B5D0BB020E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="139">
   <si>
     <t>Frame</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>Create memory map</t>
+  </si>
+  <si>
+    <t>Create chip variable</t>
+  </si>
+  <si>
+    <t>Create Priority system</t>
   </si>
 </sst>
 </file>
@@ -1694,9 +1700,9 @@
   </sheetPr>
   <dimension ref="A1:CH21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4320,10 +4326,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C443201F-21B9-4781-9C9F-956B668549C5}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4422,6 +4428,16 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed integration of memory. Added Circular Buffer for chips
</commit_message>
<xml_diff>
--- a/2. Planning and Management/Buoy Framework Development Plan.xlsx
+++ b/2. Planning and Management/Buoy Framework Development Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamie\OneDrive\Documents\GitHub\BouyDev\2. Planning and Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB84021-22F5-4DCE-A211-D0B5D0BB020E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9142A95A-768F-4251-8C15-BCD37D85B400}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{3A478CED-D59D-42F3-A5AA-7CAA389E8A3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1701,8 +1701,8 @@
   <dimension ref="A1:CH21"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18:L20"/>
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3252,7 +3252,7 @@
         <v>75</v>
       </c>
       <c r="D14" s="31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="30">
         <f>F13+1</f>
@@ -4328,7 +4328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C443201F-21B9-4781-9C9F-956B668549C5}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -4449,7 +4449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEC993A-1A13-4A33-B477-F70169CA0E29}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>

</xml_diff>